<commit_message>
-> Se añadio una función al menú para actualizar el inventario -> Se creo el método actualizar_inventario en la clase TiendaApp -> Se cambio el nombre del metodo actualizar_inventario por actualizar_inventario_venta
</commit_message>
<xml_diff>
--- a/Tienda.xlsx
+++ b/Tienda.xlsx
@@ -378,7 +378,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -410,7 +410,7 @@
         </is>
       </c>
       <c r="B2" s="5" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="5" t="inlineStr">
         <is>
@@ -440,7 +440,7 @@
         </is>
       </c>
       <c r="B4" s="5" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="B5" s="5" t="n">
-        <v>375</v>
+        <v>500</v>
       </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
@@ -470,9 +470,24 @@
         </is>
       </c>
       <c r="B6" s="5" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>unidades</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Camisa</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>36</v>
+      </c>
+      <c r="C7" t="inlineStr">
         <is>
           <t>unidades</t>
         </is>
@@ -491,7 +506,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -599,6 +614,22 @@
       </c>
       <c r="D6" s="5" t="n">
         <v>1200</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Camisa</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>35000</v>
+      </c>
+      <c r="C7" t="n">
+        <v>72000</v>
+      </c>
+      <c r="D7" t="n">
+        <v>37000</v>
       </c>
     </row>
   </sheetData>
@@ -614,7 +645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1134,6 +1165,174 @@
         <v>10000</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" s="8" t="n">
+        <v>45942</v>
+      </c>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>Loción</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="D22" s="5" t="inlineStr">
+        <is>
+          <t>gramos</t>
+        </is>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>650</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>19500</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="8" t="n">
+        <v>45942</v>
+      </c>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Chocolatina</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" s="5" t="inlineStr">
+        <is>
+          <t>unidades</t>
+        </is>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>2500</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="8" t="n">
+        <v>45942</v>
+      </c>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>Splash</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="5" t="inlineStr">
+        <is>
+          <t>unidades</t>
+        </is>
+      </c>
+      <c r="E24" s="5" t="n">
+        <v>17000</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="8" t="n">
+        <v>45942</v>
+      </c>
+      <c r="B25" s="5" t="inlineStr">
+        <is>
+          <t>Bolsa de Regalo</t>
+        </is>
+      </c>
+      <c r="C25" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" s="5" t="inlineStr">
+        <is>
+          <t>unidades</t>
+        </is>
+      </c>
+      <c r="E25" s="5" t="n">
+        <v>2500</v>
+      </c>
+      <c r="F25" s="5" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="8" t="n">
+        <v>45942</v>
+      </c>
+      <c r="B26" s="5" t="inlineStr">
+        <is>
+          <t>Splash</t>
+        </is>
+      </c>
+      <c r="C26" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D26" s="5" t="inlineStr">
+        <is>
+          <t>unidades</t>
+        </is>
+      </c>
+      <c r="E26" s="5" t="n">
+        <v>17000</v>
+      </c>
+      <c r="F26" s="5" t="n">
+        <v>34000</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="8" t="n">
+        <v>45942</v>
+      </c>
+      <c r="B27" s="5" t="inlineStr">
+        <is>
+          <t>Chocolatina</t>
+        </is>
+      </c>
+      <c r="C27" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D27" s="5" t="inlineStr">
+        <is>
+          <t>unidades</t>
+        </is>
+      </c>
+      <c r="E27" s="5" t="n">
+        <v>2500</v>
+      </c>
+      <c r="F27" s="5" t="n">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="8" t="n">
+        <v>45942</v>
+      </c>
+      <c r="B28" s="5" t="inlineStr">
+        <is>
+          <t>Loción</t>
+        </is>
+      </c>
+      <c r="C28" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="D28" s="5" t="inlineStr">
+        <is>
+          <t>gramos</t>
+        </is>
+      </c>
+      <c r="E28" s="5" t="n">
+        <v>650</v>
+      </c>
+      <c r="F28" s="5" t="n">
+        <v>65000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
-> Se añadio un metodo para ver el resumen de ventas de un dia ingresado por el usuario
</commit_message>
<xml_diff>
--- a/Tienda.xlsx
+++ b/Tienda.xlsx
@@ -463,7 +463,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -478,7 +478,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -493,7 +493,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>580</v>
+        <v>500</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -508,7 +508,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -523,7 +523,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -538,7 +538,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -694,7 +694,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1070,6 +1070,246 @@
         <v>55000</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" s="3" t="n">
+        <v>45952</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Bolsa de Regalo</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>unidades</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>3000</v>
+      </c>
+      <c r="F16" t="n">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="n">
+        <v>45952</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Loción</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>30</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>gramos</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>550</v>
+      </c>
+      <c r="F17" t="n">
+        <v>16500</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="n">
+        <v>45952</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Splash</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>unidades</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>16000</v>
+      </c>
+      <c r="F18" t="n">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="n">
+        <v>45952</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Chocolatina</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>unidades</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F19" t="n">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="n">
+        <v>45952</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Loción</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>50</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>gramos</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>550</v>
+      </c>
+      <c r="F20" t="n">
+        <v>27500</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="n">
+        <v>45952</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Chocolatina</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>unidades</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F21" t="n">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="n">
+        <v>45952</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Crema</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>3</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>unidades</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>14500</v>
+      </c>
+      <c r="F22" t="n">
+        <v>43500</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="n">
+        <v>45952</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Camisa</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>unidades</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>32000</v>
+      </c>
+      <c r="F23" t="n">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="n">
+        <v>45952</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Chocolatina</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>3</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>unidades</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F24" t="n">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="n">
+        <v>45952</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Camisa</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>unidades</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>32000</v>
+      </c>
+      <c r="F25" t="n">
+        <v>64000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
-> Se agregaron comentarios al código para mejorar la legibilidad y el mantenimiento.
</commit_message>
<xml_diff>
--- a/Tienda.xlsx
+++ b/Tienda.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,7 +523,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -538,9 +538,24 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C7" t="inlineStr">
+        <is>
+          <t>unidades</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Zapatos</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>11</v>
+      </c>
+      <c r="C8" t="inlineStr">
         <is>
           <t>unidades</t>
         </is>
@@ -557,7 +572,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -626,13 +641,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="C4" t="n">
         <v>550</v>
       </c>
       <c r="D4" t="n">
-        <v>250</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5">
@@ -681,6 +696,22 @@
       </c>
       <c r="D7" t="n">
         <v>17000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Zapatos</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>35000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>72000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>37000</v>
       </c>
     </row>
   </sheetData>
@@ -694,7 +725,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1310,6 +1341,54 @@
         <v>64000</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" s="3" t="n">
+        <v>45960</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Zapatos</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>unidades</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>72000</v>
+      </c>
+      <c r="F26" t="n">
+        <v>72000</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="n">
+        <v>45960</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Camisa</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>2</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>unidades</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>32000</v>
+      </c>
+      <c r="F27" t="n">
+        <v>64000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>